<commit_message>
vault backup: 2026-02-18 21:11:42
</commit_message>
<xml_diff>
--- a/Notes/Auth/assets/Current/Accelup requests/Accelup Improvements.xlsx
+++ b/Notes/Auth/assets/Current/Accelup requests/Accelup Improvements.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\despo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notebooks\Notebook\Notes\Auth\assets\Current\Accelup requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C5559C-F7D5-462D-9534-0DEE3A2AB695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3A4DC2-565E-42F3-9847-E7AA0A98C52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{CDCDD20E-727F-4643-AC9E-958155DFA20D}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B873939C-6C43-4D26-90F5-8038613E3245}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B873939C-6C43-4D26-90F5-8038613E3245}"/>
   </bookViews>
   <sheets>
     <sheet name="Prioritization" sheetId="4" r:id="rId1"/>
@@ -315,7 +314,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,13 +336,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κακό" xfId="2" builtinId="27"/>
+    <cellStyle name="Καλό" xfId="1" builtinId="26"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Ουδέτερο" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,15 +361,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2611406</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>92563</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752036</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -394,8 +392,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="8343900"/>
-          <a:ext cx="15346917" cy="8049748"/>
+          <a:off x="9526" y="7715250"/>
+          <a:ext cx="9257860" cy="5229225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -408,7 +406,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -726,22 +724,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31830166-A37B-42DA-BC03-BD52BC22FE63}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="1">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="113" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="50.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -757,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -765,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -773,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -781,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -789,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -797,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -805,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -813,31 +810,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -845,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -853,15 +850,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -869,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -877,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -891,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -899,7 +896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -907,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -925,19 +922,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10720D2B-12F6-4C39-8FF9-EA074B5E3A37}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="121.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="62.21875" customWidth="1"/>
+    <col min="1" max="1" width="121.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,7 +941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -954,7 +950,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -962,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -970,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -978,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -986,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -999,7 +995,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1012,7 +1008,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1021,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1038,7 +1034,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1054,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1078,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1094,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1118,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1126,7 +1122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1134,7 +1130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1142,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24">
         <f>SUM(B2:B23)</f>
         <v>62</v>
@@ -1160,18 +1156,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0EAB0F-21A2-4DEC-A621-2C11E14461C3}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="123.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="123.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1179,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1187,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1195,7 +1188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1211,7 +1204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -1227,7 +1220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1235,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -1243,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1251,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1259,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1267,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1275,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1283,7 +1276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>SUM(B2:B14)</f>
         <v>41</v>
@@ -1301,19 +1294,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508967FA-8464-4256-A653-0BA8AC26EE7D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -1324,22 +1314,22 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="74.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="74.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1347,7 +1337,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1355,17 +1345,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>

</xml_diff>